<commit_message>
Fixed DropDown issue Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>03/03/2018</t>
   </si>
   <si>
-    <t>testjaga23032018@gmail.com</t>
+    <t>testjaga18042018@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,6 +595,7 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
     <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Positive and Negative flow commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Password</t>
   </si>
@@ -86,10 +86,13 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>03/03/2018</t>
-  </si>
-  <si>
-    <t>testjaga18042018@gmail.com</t>
+    <t>jaga@1234</t>
+  </si>
+  <si>
+    <t>05/04/2018</t>
+  </si>
+  <si>
+    <t>testjaga24042018@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,15 +476,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,10 +502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +571,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -588,6 +601,47 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -595,7 +649,10 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
     <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="M3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SureFire plugin added commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testData.xlsx
+++ b/src/test/resources/TestData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Password</t>
   </si>
@@ -87,13 +87,16 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>jaga@1234</t>
-  </si>
-  <si>
     <t>05/04/2018</t>
   </si>
   <si>
     <t>testjaga24042018@gmail.com</t>
+  </si>
+  <si>
+    <t>testjaga952018@gmail.com</t>
+  </si>
+  <si>
+    <t>09/05/2018</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,19 +486,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,10 +496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -602,47 +595,6 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -650,10 +602,7 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
     <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="L3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="D2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -663,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -732,10 +681,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>

</xml_diff>